<commit_message>
Working on final json version
</commit_message>
<xml_diff>
--- a/data/paired_responses.xlsx
+++ b/data/paired_responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahojd\Documents\MIS6900\Module4_Final\hw3_hojdila\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25787FB-F869-4301-BDB8-5EFDBD434307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5536022C-D63D-408B-A7D9-E7CF4F3A0479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E5A909D9-4A88-4D34-A49A-57CF139249EF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E5A909D9-4A88-4D34-A49A-57CF139249EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>pattern</t>
   </si>
@@ -44,16 +44,40 @@
     <t>responses</t>
   </si>
   <si>
+    <t>You can find the current course website at http://www.sba.oakland.edu/faculty/isken/courses/mis6900_s24/, You can find the permalink at http://www.sba.oakland.edu/faculty/isken/courses/aap</t>
+  </si>
+  <si>
+    <t>You can find the current course website at http://www.sba.oakland.edu/faculty/isken/courses/mis5460_f23/index.html, You can find the permalink at http://www.sba.oakland.edu/faculty/isken/courses/ba</t>
+  </si>
+  <si>
+    <t>You can find the current course website at http://www.sba.oakland.edu/faculty/isken/courses/mis5470_f23/index.html, You can find the permalink at http://www.sba.oakland.edu/faculty/isken/courses/pcda</t>
+  </si>
+  <si>
+    <t>quit</t>
+  </si>
+  <si>
+    <t>mis4900</t>
+  </si>
+  <si>
+    <t>mis4460</t>
+  </si>
+  <si>
+    <t>mis4470</t>
+  </si>
+  <si>
+    <t>mis6900</t>
+  </si>
+  <si>
+    <t>mis5460</t>
+  </si>
+  <si>
+    <t>mis5470</t>
+  </si>
+  <si>
+    <t>Good bye!</t>
+  </si>
+  <si>
     <t>context_set</t>
-  </si>
-  <si>
-    <t>loaner</t>
-  </si>
-  <si>
-    <t>rental</t>
-  </si>
-  <si>
-    <t>repairs</t>
   </si>
 </sst>
 </file>
@@ -425,16 +449,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9687EDA3-045A-4DB2-AD00-810470230075}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="188.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -446,22 +468,63 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>